<commit_message>
v2.01.0 Cleared up sequence of events
</commit_message>
<xml_diff>
--- a/api/AbilityInfo.xlsx
+++ b/api/AbilityInfo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\RunescapeCalculator\api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51D2D468-4F88-48B1-B2F6-5F3FB4E1B644}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CEC97A6-185F-4089-8323-318D75E97834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="4635" windowWidth="37155" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -5525,10 +5525,10 @@
   </sheetPr>
   <dimension ref="A1:AQ111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A46" sqref="A46"/>
-      <selection pane="topRight" activeCell="C52" sqref="C52"/>
+      <selection pane="topRight" activeCell="M53" sqref="M53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -11543,10 +11543,10 @@
         <v>0</v>
       </c>
       <c r="L49" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M49" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N49" s="4">
         <v>3</v>
@@ -13194,19 +13194,19 @@
         <v>0</v>
       </c>
       <c r="L62" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M62" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N62" s="7">
         <v>0</v>
       </c>
       <c r="O62" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P62" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q62" s="4" t="s">
         <v>215</v>

</xml_diff>